<commit_message>
n-gram extraction and experimental n-gram language model are added
</commit_message>
<xml_diff>
--- a/Nuve/Resources/suffix_tr.xlsx
+++ b/Nuve/Resources/suffix_tr.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="930" windowWidth="15240" windowHeight="8070"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="724">
   <si>
     <t>Un</t>
   </si>
@@ -3104,6 +3104,9 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>bu iki ek yerine üstteki 2 eki kullanıyoruz sanırım. Emin olduktan sonra silinebilir.</t>
   </si>
 </sst>
 </file>
@@ -3162,12 +3165,18 @@
       <charset val="162"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3182,10 +3191,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3231,9 +3241,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Ofis Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Ofis">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3271,7 +3281,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Ofis">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3343,7 +3353,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Ofis">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3520,10 +3530,10 @@
   <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J55" sqref="J55"/>
+      <selection pane="bottomRight" activeCell="A55" sqref="A55:A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3537,7 +3547,7 @@
     <col min="7" max="7" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="60.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="62.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="176.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -5409,7 +5419,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -5447,7 +5457,7 @@
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -5485,7 +5495,7 @@
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -5523,7 +5533,7 @@
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -5561,7 +5571,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -5596,7 +5606,7 @@
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -5637,7 +5647,7 @@
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -5675,7 +5685,7 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -6530,6 +6540,9 @@
       <c r="I89" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="O89" s="1" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
@@ -6549,7 +6562,7 @@
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="3" t="s">
         <v>690</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -6583,11 +6596,11 @@
         <v>567</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>568</v>
+        <v>723</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="3" t="s">
         <v>659</v>
       </c>
       <c r="B92" s="1" t="s">

</xml_diff>

<commit_message>
commit before some refactoring and optimization
</commit_message>
<xml_diff>
--- a/Nuve/Resources/suffix_tr.xlsx
+++ b/Nuve/Resources/suffix_tr.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$113</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2987,21 +2987,6 @@
     <t>L_OZEL_ETTIRGEN,  L_DONUSUM_D, L_DONUSUM_U</t>
   </si>
   <si>
-    <t xml:space="preserve">yim, yum, ım, im, um, üm, m, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yin, yun, ın, in, un, ün, n, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yi, yu, sı, si, su, sü, ı, i, u, ü, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yimiz, yumuz, ımız, imiz, umuz, ümüz, mız, miz, muz, müz, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yiniz, yunuz, ınız, iniz, unuz, ünüz, nız, niz, nuz, nüz, </t>
-  </si>
-  <si>
     <t>ZAMIR_ILGI_(n)Un</t>
   </si>
   <si>
@@ -3017,18 +3002,6 @@
     <t>L_DONUSUM_A, L_DONUSUM_I, F_OZEL_N</t>
   </si>
   <si>
-    <t xml:space="preserve">yı, yi, yu, yü, ı, i, u, ü, nı, ni, nu, nü, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">de, da, te, ta, nde, nda, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">den, dan, ten, tan, nden, ndan, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">a, e, ya, ye, na, ne, </t>
-  </si>
-  <si>
     <t>F_OZEL_N</t>
   </si>
   <si>
@@ -3107,6 +3080,33 @@
   </si>
   <si>
     <t>bu iki ek yerine üstteki 2 eki kullanıyoruz sanırım. Emin olduktan sonra silinebilir.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ım, im, um, üm, m, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ın, in, un, ün, n, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sı, si, su, sü, ı, i, u, ü, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ımız, imiz, umuz, ümüz, mız, miz, muz, müz, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ınız, iniz, unuz, ünüz, nız, niz, nuz, nüz, </t>
+  </si>
+  <si>
+    <t>den, dan, ten, tan, nden, ndan</t>
+  </si>
+  <si>
+    <t>de, da, te, ta, nde, nda</t>
+  </si>
+  <si>
+    <t>yı, yi, yu, yü, ı, i, u, ü, nı, ni, nu, nü</t>
+  </si>
+  <si>
+    <t>a, e, ya, ye, na, ne</t>
   </si>
 </sst>
 </file>
@@ -3165,7 +3165,7 @@
       <charset val="162"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3175,6 +3175,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3191,11 +3197,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3530,10 +3537,10 @@
   <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A55" sqref="A55:A62"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3564,7 +3571,7 @@
         <v>297</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>298</v>
@@ -3585,7 +3592,7 @@
         <v>300</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>304</v>
@@ -3664,7 +3671,7 @@
         <v>197</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>697</v>
+        <v>715</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>354</v>
@@ -3705,7 +3712,7 @@
         <v>197</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>698</v>
+        <v>716</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>372</v>
@@ -3743,10 +3750,10 @@
         <v>356</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>699</v>
+        <v>717</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>364</v>
@@ -3787,7 +3794,7 @@
         <v>197</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>700</v>
+        <v>718</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>360</v>
@@ -3825,7 +3832,7 @@
         <v>197</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>701</v>
+        <v>719</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>376</v>
@@ -3860,7 +3867,7 @@
         <v>356</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>200</v>
@@ -3898,7 +3905,7 @@
         <v>202</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>710</v>
+        <v>723</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>349</v>
@@ -3911,7 +3918,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -3968,7 +3975,7 @@
         <v>204</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>707</v>
+        <v>722</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>331</v>
@@ -3984,7 +3991,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -4041,7 +4048,7 @@
         <v>206</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>708</v>
+        <v>721</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>335</v>
@@ -4054,7 +4061,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -4111,7 +4118,7 @@
         <v>206</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>709</v>
+        <v>720</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>321</v>
@@ -4124,7 +4131,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -4181,7 +4188,7 @@
         <v>204</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>341</v>
@@ -4251,7 +4258,7 @@
         <v>311</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>680</v>
@@ -4338,7 +4345,7 @@
         <v>654</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>688</v>
@@ -4359,7 +4366,7 @@
         <v>676</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>676</v>
@@ -4371,7 +4378,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>33</v>
@@ -5192,7 +5199,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>79</v>
@@ -5403,7 +5410,7 @@
         <v>241</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>457</v>
@@ -5412,7 +5419,7 @@
         <v>458</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
       <c r="O54" s="1" t="s">
         <v>645</v>
@@ -6474,7 +6481,7 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>52</v>
@@ -6596,7 +6603,7 @@
         <v>567</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -6823,7 +6830,7 @@
         <v>199</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>595</v>
@@ -6919,7 +6926,7 @@
         <v>287</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>605</v>
@@ -6983,7 +6990,7 @@
         <v>191</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>612</v>
@@ -7079,7 +7086,7 @@
         <v>191</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>621</v>
@@ -7131,7 +7138,7 @@
         <v>292</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>624</v>

</xml_diff>